<commit_message>
fixes #1065 - adds multiple identifier fields to spreadsheet loader and downcases creator type so it can handle capitalization
</commit_message>
<xml_diff>
--- a/spec/fixtures/files/demo_mods_new_file/manifest.xlsx
+++ b/spec/fixtures/files/demo_mods_new_file/manifest.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27224"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27309"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="201">
   <si>
     <t>What is your name?</t>
   </si>
@@ -398,9 +398,6 @@
     <t>What is the physical location for this object?</t>
   </si>
   <si>
-    <t>What is the identifier for this object?</t>
-  </si>
-  <si>
     <t>Collection Title</t>
   </si>
   <si>
@@ -600,6 +597,39 @@
   </si>
   <si>
     <t>abstract goes here</t>
+  </si>
+  <si>
+    <t>What is the original identifier?</t>
+  </si>
+  <si>
+    <t>Identifier 1</t>
+  </si>
+  <si>
+    <t>Identifier Type 1</t>
+  </si>
+  <si>
+    <t>Identifier 2</t>
+  </si>
+  <si>
+    <t>Identifier Type 2</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>Corporate</t>
+  </si>
+  <si>
+    <t>Identifier 3</t>
+  </si>
+  <si>
+    <t>Identifier Type 3</t>
+  </si>
+  <si>
+    <t>garble</t>
+  </si>
+  <si>
+    <t>archives</t>
   </si>
 </sst>
 </file>
@@ -1023,18 +1053,128 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:DC5"/>
+  <dimension ref="A1:DI5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AS1" workbookViewId="0">
-      <selection activeCell="AV4" sqref="AV4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="106" max="106" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="13" customWidth="1"/>
+    <col min="9" max="9" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="48" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="26" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="26" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="34.6640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="36.5" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="50.83203125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="15" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="36" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="11" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="50" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="9" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="16" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="8" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="37.6640625" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="88" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="33.33203125" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="32.5" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="100" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="33.33203125" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="255.83203125" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="27.5" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="53.33203125" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="27.5" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="29.1640625" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="27.5" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="32.1640625" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="27.5" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="27.5" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="39.5" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="49.5" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="18" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="28" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="39.5" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="39.83203125" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="32.83203125" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="37.6640625" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="36.5" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="46.33203125" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="26.83203125" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="46.33203125" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="26.83203125" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="33.1640625" bestFit="1" customWidth="1"/>
+    <col min="89" max="89" width="43.1640625" bestFit="1" customWidth="1"/>
+    <col min="90" max="90" width="33.1640625" bestFit="1" customWidth="1"/>
+    <col min="91" max="91" width="30.83203125" bestFit="1" customWidth="1"/>
+    <col min="92" max="92" width="41.1640625" bestFit="1" customWidth="1"/>
+    <col min="93" max="93" width="40.1640625" bestFit="1" customWidth="1"/>
+    <col min="94" max="94" width="30.83203125" bestFit="1" customWidth="1"/>
+    <col min="95" max="95" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="96" max="96" width="16" bestFit="1" customWidth="1"/>
+    <col min="97" max="97" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="98" max="98" width="44.33203125" bestFit="1" customWidth="1"/>
+    <col min="99" max="99" width="31" bestFit="1" customWidth="1"/>
+    <col min="100" max="100" width="39.6640625" bestFit="1" customWidth="1"/>
+    <col min="101" max="101" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="102" max="102" width="16" bestFit="1" customWidth="1"/>
+    <col min="103" max="103" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="104" max="104" width="44.33203125" bestFit="1" customWidth="1"/>
+    <col min="105" max="105" width="31" bestFit="1" customWidth="1"/>
+    <col min="106" max="106" width="39.6640625" bestFit="1" customWidth="1"/>
+    <col min="108" max="108" width="48" bestFit="1" customWidth="1"/>
+    <col min="109" max="109" width="33.33203125" bestFit="1" customWidth="1"/>
+    <col min="110" max="110" width="23" bestFit="1" customWidth="1"/>
+    <col min="111" max="111" width="35.33203125" bestFit="1" customWidth="1"/>
+    <col min="112" max="112" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="113" max="113" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:107" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:113" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1042,320 +1182,338 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="AF1" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="Z1" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="AH1" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="AT1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AU1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AV1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="AW1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="AX1" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="AY1" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="AZ1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="BA1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="BB1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="BC1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="BD1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="BE1" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="AC1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="AI1" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="AK1" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="AL1" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="AM1" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="AN1" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="AO1" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="AP1" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="AQ1" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="AR1" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="AS1" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="AT1" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="AU1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="AV1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AW1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="AX1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="AY1" s="2" t="s">
+      <c r="BF1" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="AZ1" s="2" t="s">
+      <c r="BG1" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="BA1" s="1" t="s">
+      <c r="BH1" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="BB1" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="BC1" s="1" t="s">
+      <c r="BI1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="BD1" s="1" t="s">
+      <c r="BJ1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="BE1" s="1" t="s">
+      <c r="BK1" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="BF1" s="1" t="s">
+      <c r="BL1" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="BG1" s="1" t="s">
+      <c r="BM1" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="BH1" s="1" t="s">
+      <c r="BN1" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="BI1" s="1" t="s">
+      <c r="BO1" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="BJ1" s="1" t="s">
+      <c r="BP1" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="BK1" s="1" t="s">
+      <c r="BQ1" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="BL1" s="1" t="s">
+      <c r="BR1" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="BM1" s="3" t="s">
+      <c r="BS1" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="BN1" s="3" t="s">
+      <c r="BT1" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="BO1" s="3" t="s">
+      <c r="BU1" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="BP1" s="3" t="s">
+      <c r="BV1" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="BQ1" s="3" t="s">
+      <c r="BW1" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="BR1" s="3" t="s">
+      <c r="BX1" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="BS1" s="3" t="s">
+      <c r="BY1" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="BT1" s="3" t="s">
+      <c r="BZ1" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="BU1" s="3" t="s">
+      <c r="CA1" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="BV1" s="1" t="s">
+      <c r="CB1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="BW1" s="1" t="s">
+      <c r="CC1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="BX1" s="1" t="s">
+      <c r="CD1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="BY1" s="1" t="s">
+      <c r="CE1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="BZ1" s="1" t="s">
+      <c r="CF1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="CA1" s="1" t="s">
+      <c r="CG1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="CB1" s="1" t="s">
+      <c r="CH1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="CC1" s="1" t="s">
+      <c r="CI1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="CD1" s="3" t="s">
+      <c r="CJ1" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="CE1" s="3" t="s">
+      <c r="CK1" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="CF1" s="3" t="s">
+      <c r="CL1" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="CG1" s="3" t="s">
+      <c r="CM1" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="CH1" s="3" t="s">
+      <c r="CN1" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="CI1" s="3" t="s">
+      <c r="CO1" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="CJ1" s="3" t="s">
+      <c r="CP1" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="CK1" s="3" t="s">
+      <c r="CQ1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="CL1" s="3" t="s">
+      <c r="CR1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="CM1" s="3" t="s">
+      <c r="CS1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="CN1" s="3" t="s">
+      <c r="CT1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="CO1" s="3" t="s">
+      <c r="CU1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="CP1" s="3" t="s">
+      <c r="CV1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="CQ1" s="3" t="s">
+      <c r="CW1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="CR1" s="3" t="s">
+      <c r="CX1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="CS1" s="3" t="s">
+      <c r="CY1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="CT1" s="3" t="s">
+      <c r="CZ1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="CU1" s="3" t="s">
+      <c r="DA1" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="CV1" s="3" t="s">
+      <c r="DB1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="CW1" s="3"/>
-      <c r="CX1" s="1" t="s">
+      <c r="DC1" s="3"/>
+      <c r="DD1" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="CY1" s="1" t="s">
+      <c r="DE1" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="CZ1" s="1" t="s">
+      <c r="DF1" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="DG1" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="DA1" s="1" t="s">
+      <c r="DH1" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="DB1" s="1" t="s">
+      <c r="DI1" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="DC1" s="1" t="s">
-        <v>126</v>
-      </c>
     </row>
-    <row r="2" spans="1:107" ht="18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:113" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>41</v>
       </c>
@@ -1366,503 +1524,527 @@
         <v>43</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>5</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>45</v>
       </c>
       <c r="L2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="X2" s="1"/>
+      <c r="Y2" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="M2" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="O2" s="1" t="s">
+      <c r="Z2" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="P2" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="R2" s="1"/>
-      <c r="S2" s="1" t="s">
+      <c r="AA2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB2" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="T2" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="V2" s="1" t="s">
+      <c r="AC2" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="W2" s="1" t="s">
+      <c r="AD2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AF2" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG2" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="AH2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI2" s="1">
+        <v>1981</v>
+      </c>
+      <c r="AJ2" s="1">
+        <v>1982</v>
+      </c>
+      <c r="AK2" s="1"/>
+      <c r="AM2" s="1">
+        <v>1982</v>
+      </c>
+      <c r="AN2" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="X2" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="Y2" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="Z2" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="AA2" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="AB2" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="AC2" s="1">
-        <v>1981</v>
-      </c>
-      <c r="AD2" s="1">
-        <v>1982</v>
-      </c>
-      <c r="AE2" s="1"/>
-      <c r="AG2" s="1">
-        <v>1982</v>
-      </c>
-      <c r="AH2" s="1" t="s">
+      <c r="AO2" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="AI2" s="1" t="s">
+      <c r="AP2" s="1"/>
+      <c r="AQ2" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="AJ2" s="1"/>
-      <c r="AK2" s="1" t="s">
+      <c r="AR2" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="AL2" s="1" t="s">
+      <c r="AS2" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="AM2" s="5" t="s">
+      <c r="AT2" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="AN2" s="1" t="s">
+      <c r="AU2" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="AO2" s="1" t="s">
+      <c r="AV2" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="AP2" s="1" t="s">
+      <c r="AW2" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="AQ2" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="AR2" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="AS2" s="1"/>
-      <c r="AT2" s="1"/>
-      <c r="AU2" s="1" t="s">
+      <c r="AX2" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="AY2" s="1"/>
+      <c r="AZ2" s="1"/>
+      <c r="BA2" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="AV2" s="1" t="s">
+      <c r="BB2" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="AW2" s="1" t="s">
+      <c r="BC2" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="AX2" s="1" t="s">
+      <c r="BD2" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="AY2" s="1" t="s">
+      <c r="BE2" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="BF2" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="BG2" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="AZ2" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="BA2" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="BB2" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="BC2" s="1" t="s">
+      <c r="BH2" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="BI2" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="BD2" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="BE2" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="BF2" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="BG2" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="BH2" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="BI2" s="1" t="s">
-        <v>143</v>
       </c>
       <c r="BJ2" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="BK2" s="1"/>
-      <c r="BL2" s="1"/>
-      <c r="BM2" s="1"/>
-      <c r="BN2" s="1"/>
-      <c r="BO2" s="1"/>
-      <c r="BP2" s="1"/>
+      <c r="BK2" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="BL2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="BM2" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="BN2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="BO2" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="BP2" s="1" t="s">
+        <v>60</v>
+      </c>
       <c r="BQ2" s="1"/>
       <c r="BR2" s="1"/>
       <c r="BS2" s="1"/>
       <c r="BT2" s="1"/>
       <c r="BU2" s="1"/>
-      <c r="BV2" s="1" t="s">
+      <c r="BV2" s="1"/>
+      <c r="BW2" s="1"/>
+      <c r="BX2" s="1"/>
+      <c r="BY2" s="1"/>
+      <c r="BZ2" s="1"/>
+      <c r="CA2" s="1"/>
+      <c r="CB2" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="BW2" s="1" t="s">
+      <c r="CC2" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="BX2" s="1" t="s">
+      <c r="CD2" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="BY2" s="1"/>
-      <c r="BZ2" s="1" t="s">
+      <c r="CE2" s="1"/>
+      <c r="CF2" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="CA2" s="1" t="s">
+      <c r="CG2" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="CB2" s="1" t="s">
+      <c r="CH2" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="CC2" s="6"/>
-      <c r="CD2" s="1"/>
-      <c r="CE2" s="1"/>
-      <c r="CF2" s="1"/>
-      <c r="CG2" s="3"/>
-      <c r="CH2" s="1"/>
-      <c r="CI2" s="1"/>
+      <c r="CI2" s="6"/>
       <c r="CJ2" s="1"/>
-      <c r="CK2" s="1" t="s">
+      <c r="CK2" s="1"/>
+      <c r="CL2" s="1"/>
+      <c r="CM2" s="3"/>
+      <c r="CN2" s="1"/>
+      <c r="CO2" s="1"/>
+      <c r="CP2" s="1"/>
+      <c r="CQ2" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="CL2" s="3" t="s">
+      <c r="CR2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="CM2" s="1" t="s">
+      <c r="CS2" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="CN2" s="1" t="s">
+      <c r="CT2" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="CO2" s="1" t="s">
+      <c r="CU2" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="CP2" s="1" t="s">
+      <c r="CV2" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="CQ2" s="1" t="s">
+      <c r="CW2" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="CR2" s="3" t="s">
+      <c r="CX2" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="CS2" s="3" t="s">
+      <c r="CY2" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="CT2" s="3" t="s">
+      <c r="CZ2" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="CU2" s="3" t="s">
+      <c r="DA2" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="CV2" s="3" t="s">
+      <c r="DB2" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="CW2" s="3"/>
-      <c r="CX2" s="1" t="s">
+      <c r="DC2" s="3"/>
+      <c r="DD2" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="CY2" s="1" t="s">
+      <c r="DE2" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="DF2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="DG2" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="CZ2" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="DA2" s="1" t="s">
+      <c r="DH2" s="7">
+        <v>42170.508518518516</v>
+      </c>
+      <c r="DI2" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="DB2" s="7">
-        <v>42170.508518518516</v>
-      </c>
-      <c r="DC2" s="1" t="s">
-        <v>146</v>
-      </c>
     </row>
-    <row r="3" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:113" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>41</v>
       </c>
       <c r="B3" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>161</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>162</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>44</v>
-      </c>
+      <c r="D3" s="8"/>
       <c r="E3" s="8"/>
-      <c r="F3" s="9"/>
+      <c r="F3" s="8"/>
       <c r="G3" s="8"/>
       <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="N3" s="8" t="s">
+      <c r="I3" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="K3" s="8"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
+      <c r="T3" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="O3" s="8" t="s">
+      <c r="U3" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="P3" s="8" t="s">
+      <c r="V3" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="Q3" s="8" t="s">
+      <c r="W3" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="R3" s="8"/>
-      <c r="S3" s="8" t="s">
+      <c r="X3" s="8"/>
+      <c r="Y3" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="Z3" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA3" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB3" s="8"/>
+      <c r="AC3" s="8"/>
+      <c r="AD3" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AE3" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="T3" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="U3" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="V3" s="8"/>
-      <c r="W3" s="8"/>
-      <c r="X3" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="Y3" s="8" t="s">
+      <c r="AF3" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG3" s="8"/>
+      <c r="AH3" s="8"/>
+      <c r="AN3" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="AO3" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="AP3" s="8"/>
+      <c r="AT3" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="AU3" s="8" t="s">
         <v>164</v>
       </c>
-      <c r="Z3" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="AA3" s="8"/>
-      <c r="AB3" s="8"/>
-      <c r="AH3" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="AI3" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="AJ3" s="8"/>
-      <c r="AN3" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="AO3" s="8" t="s">
+      <c r="AV3" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="AW3" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="AX3" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="AP3" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="AQ3" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="AR3" s="8" t="s">
+      <c r="BA3" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="BB3" s="8"/>
+      <c r="BC3" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="BD3" s="8"/>
+      <c r="BI3" s="8" t="s">
         <v>166</v>
       </c>
-      <c r="AU3" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="AV3" s="8"/>
-      <c r="AW3" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="AX3" s="8"/>
-      <c r="BC3" s="8" t="s">
+      <c r="BJ3" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="BK3" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="BD3" s="8" t="s">
+      <c r="BL3" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="BE3" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="BF3" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="BH3" s="8"/>
-      <c r="BM3" s="8"/>
       <c r="BN3" s="8"/>
-      <c r="BO3" s="8"/>
-      <c r="BP3" s="8"/>
-      <c r="BQ3" s="8"/>
-      <c r="BR3" s="8"/>
       <c r="BS3" s="8"/>
       <c r="BT3" s="8"/>
       <c r="BU3" s="8"/>
-      <c r="BV3" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="BW3" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="BX3" s="8" t="s">
-        <v>62</v>
-      </c>
+      <c r="BV3" s="8"/>
+      <c r="BW3" s="8"/>
+      <c r="BX3" s="8"/>
       <c r="BY3" s="8"/>
-      <c r="BZ3" s="10" t="s">
-        <v>170</v>
-      </c>
+      <c r="BZ3" s="8"/>
       <c r="CA3" s="8"/>
       <c r="CB3" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="CC3" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="CD3" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="CE3" s="8"/>
+      <c r="CF3" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="CG3" s="8"/>
+      <c r="CH3" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="CD3" s="9"/>
-      <c r="CX3" s="8" t="s">
+      <c r="CJ3" s="9"/>
+      <c r="DD3" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="DE3" s="8" t="s">
         <v>171</v>
       </c>
-      <c r="CY3" s="8" t="s">
+      <c r="DF3" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="CZ3" s="8" t="s">
+      <c r="DG3" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="DH3" s="11">
+        <v>42285.597905092596</v>
+      </c>
+      <c r="DI3" s="8" t="s">
         <v>173</v>
       </c>
-      <c r="DA3" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="DB3" s="11">
-        <v>42285.597905092596</v>
-      </c>
-      <c r="DC3" s="8" t="s">
-        <v>174</v>
-      </c>
     </row>
-    <row r="4" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:113" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>41</v>
       </c>
       <c r="B4" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>175</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>44</v>
-      </c>
+      <c r="D4" s="8"/>
       <c r="E4" s="8"/>
-      <c r="F4" s="8" t="s">
-        <v>177</v>
-      </c>
+      <c r="F4" s="8"/>
       <c r="G4" s="8"/>
       <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="N4" s="8" t="s">
+      <c r="I4" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="M4" s="8"/>
+      <c r="N4" s="8"/>
+      <c r="O4" s="8"/>
+      <c r="P4" s="8"/>
+      <c r="T4" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="O4" s="8" t="s">
+      <c r="U4" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="P4" s="8" t="s">
+      <c r="V4" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="Q4" s="8" t="s">
+      <c r="W4" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="R4" s="8"/>
-      <c r="S4" s="8" t="s">
-        <v>163</v>
-      </c>
-      <c r="T4" s="8" t="s">
+      <c r="X4" s="8"/>
+      <c r="Y4" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="Z4" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="U4" s="8" t="s">
+      <c r="AA4" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="V4" s="8"/>
-      <c r="W4" s="8"/>
-      <c r="X4" s="8" t="s">
+      <c r="AB4" s="8"/>
+      <c r="AC4" s="8"/>
+      <c r="AD4" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="Y4" s="8" t="s">
+      <c r="AE4" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="AF4" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG4" s="8"/>
+      <c r="AH4" s="8"/>
+      <c r="AN4" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="AO4" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="AP4" s="8"/>
+      <c r="AT4" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="AU4" s="8" t="s">
         <v>178</v>
       </c>
-      <c r="Z4" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="AA4" s="8"/>
-      <c r="AB4" s="8"/>
-      <c r="AH4" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="AI4" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="AJ4" s="8"/>
-      <c r="AN4" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="AO4" s="8" t="s">
+      <c r="AV4" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="AW4" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="AX4" s="8" t="s">
         <v>179</v>
       </c>
-      <c r="AP4" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="AQ4" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="AR4" s="8" t="s">
-        <v>180</v>
-      </c>
-      <c r="AU4" s="8" t="s">
+      <c r="BA4" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="AV4" s="8"/>
-      <c r="AW4" s="8" t="s">
+      <c r="BB4" s="8"/>
+      <c r="BC4" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="AX4" s="8"/>
-      <c r="BC4" s="8"/>
       <c r="BD4" s="8"/>
-      <c r="BE4" s="8"/>
-      <c r="BF4" s="8"/>
-      <c r="BH4" s="8"/>
-      <c r="BM4" s="8"/>
+      <c r="BI4" s="8"/>
+      <c r="BJ4" s="8"/>
+      <c r="BK4" s="8"/>
+      <c r="BL4" s="8"/>
       <c r="BN4" s="8"/>
-      <c r="BO4" s="8"/>
-      <c r="BP4" s="8"/>
-      <c r="BQ4" s="8"/>
-      <c r="BR4" s="8"/>
       <c r="BS4" s="8"/>
       <c r="BT4" s="8"/>
       <c r="BU4" s="8"/>
@@ -1870,187 +2052,201 @@
       <c r="BW4" s="8"/>
       <c r="BX4" s="8"/>
       <c r="BY4" s="8"/>
-      <c r="BZ4" s="10"/>
+      <c r="BZ4" s="8"/>
       <c r="CA4" s="8"/>
       <c r="CB4" s="8"/>
-      <c r="CD4" s="9"/>
-      <c r="CX4" s="8" t="s">
-        <v>177</v>
-      </c>
-      <c r="CY4" s="8" t="s">
-        <v>172</v>
-      </c>
-      <c r="CZ4" s="8" t="s">
+      <c r="CC4" s="8"/>
+      <c r="CD4" s="8"/>
+      <c r="CE4" s="8"/>
+      <c r="CF4" s="10"/>
+      <c r="CG4" s="8"/>
+      <c r="CH4" s="8"/>
+      <c r="CJ4" s="9"/>
+      <c r="DD4" s="8" t="s">
         <v>176</v>
       </c>
-      <c r="DA4" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="DB4" s="11">
+      <c r="DE4" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="DF4" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="DG4" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="DH4" s="11">
         <v>42285.606759259259</v>
       </c>
-      <c r="DC4" s="8" t="s">
-        <v>174</v>
+      <c r="DI4" s="8" t="s">
+        <v>173</v>
       </c>
     </row>
-    <row r="5" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:113" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
         <v>41</v>
       </c>
       <c r="B5" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="C5" s="8" t="s">
         <v>181</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>182</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>44</v>
-      </c>
+      <c r="D5" s="8"/>
       <c r="E5" s="8"/>
-      <c r="F5" s="8" t="s">
-        <v>183</v>
-      </c>
+      <c r="F5" s="8"/>
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-      <c r="N5" s="8" t="s">
+      <c r="I5" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8"/>
+      <c r="O5" s="8"/>
+      <c r="P5" s="8"/>
+      <c r="T5" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="U5" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="V5" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="W5" s="8" t="s">
         <v>184</v>
       </c>
-      <c r="O5" s="8" t="s">
+      <c r="X5" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="Y5" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="Z5" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="P5" s="8" t="s">
+      <c r="AA5" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="Q5" s="8" t="s">
-        <v>185</v>
-      </c>
-      <c r="R5" s="8" t="s">
+      <c r="AB5" s="8"/>
+      <c r="AC5" s="8"/>
+      <c r="AD5" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AE5" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="AF5" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG5" s="8"/>
+      <c r="AH5" s="8"/>
+      <c r="AN5" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="AO5" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="AP5" s="8"/>
+      <c r="AT5" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="AU5" s="8" t="s">
         <v>186</v>
       </c>
-      <c r="S5" s="8" t="s">
-        <v>163</v>
-      </c>
-      <c r="T5" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="U5" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="V5" s="8"/>
-      <c r="W5" s="8"/>
-      <c r="X5" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="Y5" s="8" t="s">
-        <v>178</v>
-      </c>
-      <c r="Z5" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="AA5" s="8"/>
-      <c r="AB5" s="8"/>
-      <c r="AH5" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="AI5" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="AJ5" s="8"/>
-      <c r="AN5" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="AO5" s="8" t="s">
+      <c r="AV5" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="AW5" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="AX5" s="8" t="s">
         <v>187</v>
       </c>
-      <c r="AP5" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="AQ5" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="AR5" s="8" t="s">
+      <c r="BA5" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="BB5" s="8"/>
+      <c r="BC5" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="BD5" s="8"/>
+      <c r="BI5" s="8" t="s">
         <v>188</v>
       </c>
-      <c r="AU5" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="AV5" s="8"/>
-      <c r="AW5" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="AX5" s="8"/>
-      <c r="BC5" s="8" t="s">
-        <v>189</v>
-      </c>
-      <c r="BD5" s="8" t="s">
+      <c r="BJ5" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="BE5" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="BF5" s="8" t="s">
+      <c r="BK5" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="BL5" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="BH5" s="8"/>
-      <c r="BM5" s="8"/>
       <c r="BN5" s="8"/>
-      <c r="BO5" s="8"/>
-      <c r="BP5" s="8"/>
-      <c r="BQ5" s="8"/>
-      <c r="BR5" s="8"/>
       <c r="BS5" s="8"/>
       <c r="BT5" s="8"/>
       <c r="BU5" s="8"/>
-      <c r="BV5" s="8" t="s">
+      <c r="BV5" s="8"/>
+      <c r="BW5" s="8"/>
+      <c r="BX5" s="8"/>
+      <c r="BY5" s="8"/>
+      <c r="BZ5" s="8"/>
+      <c r="CA5" s="8"/>
+      <c r="CB5" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="BW5" s="8" t="s">
+      <c r="CC5" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="BX5" s="8" t="s">
+      <c r="CD5" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="BY5" s="8"/>
-      <c r="BZ5" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="CA5" s="8" t="s">
+      <c r="CE5" s="8"/>
+      <c r="CF5" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="CG5" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="CB5" s="8" t="s">
+      <c r="CH5" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="CD5" s="9"/>
-      <c r="CX5" s="8" t="s">
-        <v>183</v>
-      </c>
-      <c r="CY5" s="8" t="s">
-        <v>172</v>
-      </c>
-      <c r="CZ5" s="8" t="s">
+      <c r="CJ5" s="9"/>
+      <c r="DD5" s="8" t="s">
         <v>182</v>
       </c>
-      <c r="DA5" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="DB5" s="11">
+      <c r="DE5" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="DF5" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="DG5" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="DH5" s="11">
         <v>42285.616435185184</v>
       </c>
-      <c r="DC5" s="8" t="s">
-        <v>174</v>
+      <c r="DI5" s="8" t="s">
+        <v>173</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="AX2:AZ2">
+  <conditionalFormatting sqref="BD2:BF2">
     <cfRule type="notContainsBlanks" dxfId="1" priority="2">
-      <formula>LEN(TRIM(AX2))&gt;0</formula>
+      <formula>LEN(TRIM(BD2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AW2">
+  <conditionalFormatting sqref="BC2">
     <cfRule type="notContainsBlanks" dxfId="0" priority="1">
-      <formula>LEN(TRIM(AW2))&gt;0</formula>
+      <formula>LEN(TRIM(BC2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>